<commit_message>
Madhuri Ghute solved admin side defects
</commit_message>
<xml_diff>
--- a/WebApp/admin/public/BulkUploadTemplates/Product Insert Template.xlsx
+++ b/WebApp/admin/public/BulkUploadTemplates/Product Insert Template.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$115</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$X$115</definedName>
   </definedNames>
   <calcPr calcId="144525" iterateDelta="1E-4"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>section</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>size</t>
-  </si>
-  <si>
-    <t>color</t>
   </si>
   <si>
     <t>tags</t>
@@ -769,7 +766,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -777,11 +774,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AME115"/>
+  <dimension ref="A1:AMD115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -801,27 +798,27 @@
     <col min="13" max="13" width="21.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" style="7"/>
-    <col min="18" max="18" width="11.42578125" style="7" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" style="7" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" style="7" customWidth="1"/>
-    <col min="25" max="25" width="11.85546875" style="7" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="7"/>
+    <col min="16" max="16" width="9.140625" style="7"/>
+    <col min="17" max="17" width="11.42578125" style="7" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" style="7" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" style="7" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" style="7" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1019" s="25" customFormat="1" ht="50.45" customHeight="1">
+    <row r="1" spans="1:1018" s="25" customFormat="1" ht="50.45" customHeight="1">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>1</v>
@@ -839,7 +836,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J1" s="22" t="s">
         <v>6</v>
@@ -878,52 +875,49 @@
         <v>17</v>
       </c>
       <c r="V1" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" s="22" t="s">
         <v>18</v>
-      </c>
-      <c r="W1" s="22" t="s">
-        <v>41</v>
       </c>
       <c r="X1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="22" t="s">
-        <v>20</v>
-      </c>
+      <c r="Y1" s="24"/>
       <c r="Z1" s="24"/>
       <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
+      <c r="ALY1" s="24"/>
       <c r="ALZ1" s="24"/>
       <c r="AMA1" s="24"/>
       <c r="AMB1" s="24"/>
       <c r="AMC1" s="24"/>
       <c r="AMD1" s="24"/>
-      <c r="AME1" s="24"/>
-    </row>
-    <row r="2" spans="1:1019" ht="82.5" customHeight="1">
+    </row>
+    <row r="2" spans="1:1018" ht="82.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="2">
         <v>1001</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J2" s="1">
         <v>500</v>
@@ -938,63 +932,62 @@
         <v>100</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1">
         <v>6</v>
       </c>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="T2" s="1">
+      <c r="Q2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="1">
         <v>0</v>
       </c>
+      <c r="T2" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="U2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y2" s="1">
+        <v>38</v>
+      </c>
+      <c r="X2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1019" ht="63.75">
+    <row r="3" spans="1:1018" ht="63.75">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2">
         <v>1002</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="1">
         <v>180</v>
@@ -1009,39 +1002,38 @@
         <v>100</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1">
         <v>6</v>
       </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="T3" s="1">
+      <c r="Q3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="1">
         <v>0</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="U3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="V3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>43</v>
+      <c r="V3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0</v>
       </c>
       <c r="X3" s="1">
         <v>0</v>
       </c>
-      <c r="Y3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1019">
+    </row>
+    <row r="4" spans="1:1018">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1059,16 +1051,15 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="1"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="6"/>
       <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
+      <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-    </row>
-    <row r="5" spans="1:1019">
+    </row>
+    <row r="5" spans="1:1018">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1086,16 +1077,15 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="1"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="6"/>
       <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
+      <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-    </row>
-    <row r="6" spans="1:1019">
+    </row>
+    <row r="6" spans="1:1018">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1113,16 +1103,15 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="1"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="6"/>
       <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
+      <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-    </row>
-    <row r="7" spans="1:1019">
+    </row>
+    <row r="7" spans="1:1018">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1139,17 +1128,16 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="1"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="6"/>
       <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
+      <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-    </row>
-    <row r="8" spans="1:1019" ht="95.25" customHeight="1">
+    </row>
+    <row r="8" spans="1:1018" ht="95.25" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1167,16 +1155,15 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="1"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="6"/>
       <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
+      <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-    </row>
-    <row r="9" spans="1:1019">
+    </row>
+    <row r="9" spans="1:1018">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1194,16 +1181,15 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="1"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="6"/>
       <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
+      <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-    </row>
-    <row r="10" spans="1:1019">
+    </row>
+    <row r="10" spans="1:1018">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1221,16 +1207,15 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="1"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="6"/>
       <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
+      <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-    </row>
-    <row r="11" spans="1:1019">
+    </row>
+    <row r="11" spans="1:1018">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1248,16 +1233,15 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="1"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="6"/>
       <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
+      <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-    </row>
-    <row r="12" spans="1:1019">
+    </row>
+    <row r="12" spans="1:1018">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1275,16 +1259,15 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="1"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="6"/>
       <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
+      <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-    </row>
-    <row r="13" spans="1:1019">
+    </row>
+    <row r="13" spans="1:1018">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1302,16 +1285,15 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="1"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="6"/>
       <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
+      <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-    </row>
-    <row r="14" spans="1:1019">
+    </row>
+    <row r="14" spans="1:1018">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1329,16 +1311,15 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="1"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="6"/>
       <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
+      <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-    </row>
-    <row r="15" spans="1:1019">
+    </row>
+    <row r="15" spans="1:1018">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1356,16 +1337,15 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="1"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="6"/>
       <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
+      <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-    </row>
-    <row r="16" spans="1:1019">
+    </row>
+    <row r="16" spans="1:1018">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1383,16 +1363,15 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="1"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="6"/>
       <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
+      <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-    </row>
-    <row r="17" spans="1:25">
+    </row>
+    <row r="17" spans="1:24">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1410,16 +1389,15 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="1"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="6"/>
       <c r="U17" s="6"/>
-      <c r="V17" s="6"/>
+      <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-    </row>
-    <row r="18" spans="1:25">
+    </row>
+    <row r="18" spans="1:24">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1437,16 +1415,15 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="1"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="6"/>
       <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
+      <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-    </row>
-    <row r="19" spans="1:25">
+    </row>
+    <row r="19" spans="1:24">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1466,14 +1443,13 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
+      <c r="T19" s="6"/>
       <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
+      <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-    </row>
-    <row r="20" spans="1:25">
+    </row>
+    <row r="20" spans="1:24">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1491,16 +1467,15 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="1"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="6"/>
       <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
+      <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-    </row>
-    <row r="21" spans="1:25">
+    </row>
+    <row r="21" spans="1:24">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1518,16 +1493,15 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="1"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="6"/>
       <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
+      <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-    </row>
-    <row r="22" spans="1:25">
+    </row>
+    <row r="22" spans="1:24">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1545,16 +1519,15 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="1"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="6"/>
       <c r="U22" s="6"/>
-      <c r="V22" s="6"/>
+      <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-    </row>
-    <row r="23" spans="1:25">
+    </row>
+    <row r="23" spans="1:24">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1572,16 +1545,15 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="1"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="6"/>
       <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
+      <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-    </row>
-    <row r="24" spans="1:25">
+    </row>
+    <row r="24" spans="1:24">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1599,16 +1571,15 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="1"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="6"/>
       <c r="U24" s="6"/>
-      <c r="V24" s="6"/>
+      <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-    </row>
-    <row r="25" spans="1:25">
+    </row>
+    <row r="25" spans="1:24">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1626,16 +1597,15 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="6"/>
-      <c r="T25" s="1"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="6"/>
       <c r="U25" s="6"/>
-      <c r="V25" s="6"/>
+      <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-    </row>
-    <row r="26" spans="1:25">
+    </row>
+    <row r="26" spans="1:24">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1653,16 +1623,15 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="1"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="6"/>
       <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
+      <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-    </row>
-    <row r="27" spans="1:25" ht="114.75" customHeight="1">
+    </row>
+    <row r="27" spans="1:24" ht="114.75" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1680,16 +1649,15 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="1"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="6"/>
       <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
+      <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-    </row>
-    <row r="28" spans="1:25">
+    </row>
+    <row r="28" spans="1:24">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1707,16 +1675,15 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="1"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="6"/>
       <c r="U28" s="6"/>
-      <c r="V28" s="6"/>
+      <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-    </row>
-    <row r="29" spans="1:25">
+    </row>
+    <row r="29" spans="1:24">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1734,16 +1701,15 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="1"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="6"/>
       <c r="U29" s="6"/>
-      <c r="V29" s="6"/>
+      <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-    </row>
-    <row r="30" spans="1:25">
+    </row>
+    <row r="30" spans="1:24">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1761,16 +1727,15 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="1"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="6"/>
       <c r="U30" s="6"/>
-      <c r="V30" s="6"/>
+      <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
-    </row>
-    <row r="31" spans="1:25">
+    </row>
+    <row r="31" spans="1:24">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1788,16 +1753,15 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="6"/>
-      <c r="T31" s="1"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="6"/>
       <c r="U31" s="6"/>
-      <c r="V31" s="6"/>
+      <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-    </row>
-    <row r="32" spans="1:25">
+    </row>
+    <row r="32" spans="1:24">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1815,16 +1779,15 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="6"/>
-      <c r="T32" s="1"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="6"/>
       <c r="U32" s="6"/>
-      <c r="V32" s="6"/>
+      <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
-      <c r="Y32" s="1"/>
-    </row>
-    <row r="33" spans="1:25">
+    </row>
+    <row r="33" spans="1:24">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1842,16 +1805,15 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="6"/>
-      <c r="T33" s="1"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="6"/>
       <c r="U33" s="6"/>
-      <c r="V33" s="6"/>
+      <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-    </row>
-    <row r="34" spans="1:25">
+    </row>
+    <row r="34" spans="1:24">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1869,16 +1831,15 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="6"/>
-      <c r="T34" s="1"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="6"/>
       <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
+      <c r="V34" s="1"/>
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
-      <c r="Y34" s="1"/>
-    </row>
-    <row r="35" spans="1:25" ht="87" customHeight="1">
+    </row>
+    <row r="35" spans="1:24" ht="87" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1896,16 +1857,15 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="6"/>
-      <c r="T35" s="1"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="6"/>
       <c r="U35" s="6"/>
-      <c r="V35" s="6"/>
+      <c r="V35" s="1"/>
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
-      <c r="Y35" s="1"/>
-    </row>
-    <row r="36" spans="1:25">
+    </row>
+    <row r="36" spans="1:24">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1923,16 +1883,15 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="1"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="6"/>
       <c r="U36" s="6"/>
-      <c r="V36" s="6"/>
+      <c r="V36" s="1"/>
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
-      <c r="Y36" s="1"/>
-    </row>
-    <row r="37" spans="1:25">
+    </row>
+    <row r="37" spans="1:24">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1950,16 +1909,15 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="6"/>
-      <c r="T37" s="1"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="6"/>
       <c r="U37" s="6"/>
-      <c r="V37" s="6"/>
+      <c r="V37" s="1"/>
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
-      <c r="Y37" s="1"/>
-    </row>
-    <row r="38" spans="1:25">
+    </row>
+    <row r="38" spans="1:24">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1977,16 +1935,15 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="6"/>
-      <c r="T38" s="1"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="6"/>
       <c r="U38" s="6"/>
-      <c r="V38" s="6"/>
+      <c r="V38" s="1"/>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
-      <c r="Y38" s="1"/>
-    </row>
-    <row r="39" spans="1:25">
+    </row>
+    <row r="39" spans="1:24">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2004,16 +1961,15 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="6"/>
-      <c r="T39" s="1"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="6"/>
       <c r="U39" s="6"/>
-      <c r="V39" s="6"/>
+      <c r="V39" s="1"/>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
-      <c r="Y39" s="1"/>
-    </row>
-    <row r="40" spans="1:25">
+    </row>
+    <row r="40" spans="1:24">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2031,16 +1987,15 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-      <c r="S40" s="6"/>
-      <c r="T40" s="1"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="6"/>
       <c r="U40" s="6"/>
-      <c r="V40" s="6"/>
+      <c r="V40" s="1"/>
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
-      <c r="Y40" s="1"/>
-    </row>
-    <row r="41" spans="1:25">
+    </row>
+    <row r="41" spans="1:24">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2058,16 +2013,15 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
-      <c r="S41" s="6"/>
-      <c r="T41" s="1"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="6"/>
       <c r="U41" s="6"/>
-      <c r="V41" s="6"/>
+      <c r="V41" s="1"/>
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
-      <c r="Y41" s="1"/>
-    </row>
-    <row r="42" spans="1:25" ht="99" customHeight="1">
+    </row>
+    <row r="42" spans="1:24" ht="99" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2085,16 +2039,15 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="6"/>
-      <c r="T42" s="1"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="6"/>
       <c r="U42" s="6"/>
-      <c r="V42" s="6"/>
+      <c r="V42" s="1"/>
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
-      <c r="Y42" s="1"/>
-    </row>
-    <row r="43" spans="1:25" ht="130.5" customHeight="1">
+    </row>
+    <row r="43" spans="1:24" ht="130.5" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2112,16 +2065,15 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
-      <c r="S43" s="6"/>
-      <c r="T43" s="1"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="6"/>
       <c r="U43" s="6"/>
-      <c r="V43" s="6"/>
+      <c r="V43" s="1"/>
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
-      <c r="Y43" s="1"/>
-    </row>
-    <row r="44" spans="1:25">
+    </row>
+    <row r="44" spans="1:24">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2139,16 +2091,15 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
-      <c r="S44" s="6"/>
-      <c r="T44" s="1"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="6"/>
       <c r="U44" s="6"/>
-      <c r="V44" s="6"/>
+      <c r="V44" s="1"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
-      <c r="Y44" s="1"/>
-    </row>
-    <row r="45" spans="1:25">
+    </row>
+    <row r="45" spans="1:24">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2166,16 +2117,15 @@
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
-      <c r="R45" s="1"/>
-      <c r="S45" s="6"/>
-      <c r="T45" s="1"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="6"/>
       <c r="U45" s="6"/>
-      <c r="V45" s="6"/>
+      <c r="V45" s="1"/>
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
-      <c r="Y45" s="1"/>
-    </row>
-    <row r="46" spans="1:25">
+    </row>
+    <row r="46" spans="1:24">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2193,16 +2143,15 @@
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
-      <c r="S46" s="6"/>
-      <c r="T46" s="1"/>
+      <c r="R46" s="6"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="6"/>
       <c r="U46" s="6"/>
-      <c r="V46" s="6"/>
+      <c r="V46" s="1"/>
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
-      <c r="Y46" s="1"/>
-    </row>
-    <row r="47" spans="1:25">
+    </row>
+    <row r="47" spans="1:24">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2220,16 +2169,15 @@
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
-      <c r="S47" s="6"/>
-      <c r="T47" s="1"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="6"/>
       <c r="U47" s="6"/>
-      <c r="V47" s="6"/>
+      <c r="V47" s="1"/>
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
-      <c r="Y47" s="1"/>
-    </row>
-    <row r="48" spans="1:25">
+    </row>
+    <row r="48" spans="1:24">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2247,16 +2195,15 @@
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
-      <c r="S48" s="6"/>
-      <c r="T48" s="1"/>
+      <c r="R48" s="6"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="6"/>
       <c r="U48" s="6"/>
-      <c r="V48" s="6"/>
+      <c r="V48" s="1"/>
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
-      <c r="Y48" s="1"/>
-    </row>
-    <row r="49" spans="1:25">
+    </row>
+    <row r="49" spans="1:24">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2274,16 +2221,15 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
-      <c r="S49" s="6"/>
-      <c r="T49" s="1"/>
+      <c r="R49" s="6"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="6"/>
       <c r="U49" s="6"/>
-      <c r="V49" s="6"/>
+      <c r="V49" s="1"/>
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
-      <c r="Y49" s="1"/>
-    </row>
-    <row r="50" spans="1:25">
+    </row>
+    <row r="50" spans="1:24">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2301,16 +2247,15 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
-      <c r="S50" s="6"/>
-      <c r="T50" s="1"/>
+      <c r="R50" s="6"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="6"/>
       <c r="U50" s="6"/>
-      <c r="V50" s="6"/>
+      <c r="V50" s="1"/>
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
-      <c r="Y50" s="1"/>
-    </row>
-    <row r="51" spans="1:25">
+    </row>
+    <row r="51" spans="1:24">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2328,16 +2273,15 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
-      <c r="R51" s="1"/>
-      <c r="S51" s="6"/>
-      <c r="T51" s="1"/>
+      <c r="R51" s="6"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="6"/>
       <c r="U51" s="6"/>
-      <c r="V51" s="6"/>
+      <c r="V51" s="1"/>
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
-      <c r="Y51" s="1"/>
-    </row>
-    <row r="52" spans="1:25">
+    </row>
+    <row r="52" spans="1:24">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2355,16 +2299,15 @@
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
-      <c r="S52" s="6"/>
-      <c r="T52" s="1"/>
+      <c r="R52" s="6"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="6"/>
       <c r="U52" s="6"/>
-      <c r="V52" s="6"/>
+      <c r="V52" s="1"/>
       <c r="W52" s="1"/>
       <c r="X52" s="1"/>
-      <c r="Y52" s="1"/>
-    </row>
-    <row r="53" spans="1:25">
+    </row>
+    <row r="53" spans="1:24">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2382,16 +2325,15 @@
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
-      <c r="S53" s="6"/>
-      <c r="T53" s="1"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="6"/>
       <c r="U53" s="6"/>
-      <c r="V53" s="6"/>
+      <c r="V53" s="1"/>
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
-      <c r="Y53" s="1"/>
-    </row>
-    <row r="54" spans="1:25">
+    </row>
+    <row r="54" spans="1:24">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2409,16 +2351,15 @@
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
-      <c r="S54" s="6"/>
-      <c r="T54" s="1"/>
+      <c r="R54" s="6"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="6"/>
       <c r="U54" s="6"/>
-      <c r="V54" s="6"/>
+      <c r="V54" s="1"/>
       <c r="W54" s="1"/>
       <c r="X54" s="1"/>
-      <c r="Y54" s="1"/>
-    </row>
-    <row r="55" spans="1:25">
+    </row>
+    <row r="55" spans="1:24">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2436,16 +2377,15 @@
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
-      <c r="R55" s="1"/>
-      <c r="S55" s="6"/>
-      <c r="T55" s="1"/>
+      <c r="R55" s="6"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="6"/>
       <c r="U55" s="6"/>
-      <c r="V55" s="6"/>
+      <c r="V55" s="1"/>
       <c r="W55" s="1"/>
       <c r="X55" s="1"/>
-      <c r="Y55" s="1"/>
-    </row>
-    <row r="56" spans="1:25">
+    </row>
+    <row r="56" spans="1:24">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2463,16 +2403,15 @@
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
-      <c r="S56" s="6"/>
-      <c r="T56" s="1"/>
+      <c r="R56" s="6"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="6"/>
       <c r="U56" s="6"/>
-      <c r="V56" s="6"/>
+      <c r="V56" s="1"/>
       <c r="W56" s="1"/>
       <c r="X56" s="1"/>
-      <c r="Y56" s="1"/>
-    </row>
-    <row r="57" spans="1:25">
+    </row>
+    <row r="57" spans="1:24">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2490,16 +2429,15 @@
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
-      <c r="S57" s="6"/>
-      <c r="T57" s="1"/>
+      <c r="R57" s="6"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="6"/>
       <c r="U57" s="6"/>
-      <c r="V57" s="6"/>
+      <c r="V57" s="1"/>
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
-      <c r="Y57" s="1"/>
-    </row>
-    <row r="58" spans="1:25">
+    </row>
+    <row r="58" spans="1:24">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2517,16 +2455,15 @@
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
-      <c r="S58" s="6"/>
-      <c r="T58" s="1"/>
+      <c r="R58" s="6"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="6"/>
       <c r="U58" s="6"/>
-      <c r="V58" s="6"/>
+      <c r="V58" s="1"/>
       <c r="W58" s="1"/>
       <c r="X58" s="1"/>
-      <c r="Y58" s="1"/>
-    </row>
-    <row r="59" spans="1:25">
+    </row>
+    <row r="59" spans="1:24">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2544,16 +2481,15 @@
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
-      <c r="R59" s="1"/>
-      <c r="S59" s="6"/>
-      <c r="T59" s="1"/>
+      <c r="R59" s="6"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="6"/>
       <c r="U59" s="6"/>
-      <c r="V59" s="6"/>
+      <c r="V59" s="1"/>
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
-      <c r="Y59" s="1"/>
-    </row>
-    <row r="60" spans="1:25">
+    </row>
+    <row r="60" spans="1:24">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2571,16 +2507,15 @@
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
-      <c r="R60" s="1"/>
-      <c r="S60" s="6"/>
-      <c r="T60" s="1"/>
+      <c r="R60" s="6"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="6"/>
       <c r="U60" s="6"/>
-      <c r="V60" s="6"/>
+      <c r="V60" s="1"/>
       <c r="W60" s="1"/>
       <c r="X60" s="1"/>
-      <c r="Y60" s="1"/>
-    </row>
-    <row r="61" spans="1:25">
+    </row>
+    <row r="61" spans="1:24">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2598,16 +2533,15 @@
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
-      <c r="S61" s="6"/>
-      <c r="T61" s="1"/>
+      <c r="R61" s="6"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="6"/>
       <c r="U61" s="6"/>
-      <c r="V61" s="6"/>
+      <c r="V61" s="1"/>
       <c r="W61" s="1"/>
       <c r="X61" s="1"/>
-      <c r="Y61" s="1"/>
-    </row>
-    <row r="62" spans="1:25">
+    </row>
+    <row r="62" spans="1:24">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2625,16 +2559,15 @@
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
-      <c r="S62" s="6"/>
-      <c r="T62" s="1"/>
+      <c r="R62" s="6"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="6"/>
       <c r="U62" s="6"/>
-      <c r="V62" s="6"/>
+      <c r="V62" s="1"/>
       <c r="W62" s="1"/>
       <c r="X62" s="1"/>
-      <c r="Y62" s="1"/>
-    </row>
-    <row r="63" spans="1:25">
+    </row>
+    <row r="63" spans="1:24">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2652,16 +2585,15 @@
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
-      <c r="R63" s="1"/>
-      <c r="S63" s="6"/>
-      <c r="T63" s="1"/>
+      <c r="R63" s="6"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="6"/>
       <c r="U63" s="6"/>
-      <c r="V63" s="6"/>
+      <c r="V63" s="1"/>
       <c r="W63" s="1"/>
       <c r="X63" s="1"/>
-      <c r="Y63" s="1"/>
-    </row>
-    <row r="64" spans="1:25">
+    </row>
+    <row r="64" spans="1:24">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2679,16 +2611,15 @@
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
-      <c r="S64" s="6"/>
-      <c r="T64" s="1"/>
+      <c r="R64" s="6"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="6"/>
       <c r="U64" s="6"/>
-      <c r="V64" s="6"/>
+      <c r="V64" s="1"/>
       <c r="W64" s="1"/>
       <c r="X64" s="1"/>
-      <c r="Y64" s="1"/>
-    </row>
-    <row r="65" spans="1:25">
+    </row>
+    <row r="65" spans="1:24">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2706,16 +2637,15 @@
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
-      <c r="S65" s="6"/>
-      <c r="T65" s="1"/>
+      <c r="R65" s="6"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="6"/>
       <c r="U65" s="6"/>
-      <c r="V65" s="6"/>
+      <c r="V65" s="1"/>
       <c r="W65" s="1"/>
       <c r="X65" s="1"/>
-      <c r="Y65" s="1"/>
-    </row>
-    <row r="66" spans="1:25">
+    </row>
+    <row r="66" spans="1:24">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2733,16 +2663,15 @@
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
-      <c r="R66" s="1"/>
-      <c r="S66" s="6"/>
-      <c r="T66" s="1"/>
+      <c r="R66" s="6"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="6"/>
       <c r="U66" s="6"/>
-      <c r="V66" s="6"/>
+      <c r="V66" s="1"/>
       <c r="W66" s="1"/>
       <c r="X66" s="1"/>
-      <c r="Y66" s="1"/>
-    </row>
-    <row r="67" spans="1:25">
+    </row>
+    <row r="67" spans="1:24">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2760,16 +2689,15 @@
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-      <c r="S67" s="6"/>
-      <c r="T67" s="1"/>
+      <c r="R67" s="6"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="6"/>
       <c r="U67" s="6"/>
-      <c r="V67" s="6"/>
+      <c r="V67" s="1"/>
       <c r="W67" s="1"/>
       <c r="X67" s="1"/>
-      <c r="Y67" s="1"/>
-    </row>
-    <row r="68" spans="1:25">
+    </row>
+    <row r="68" spans="1:24">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2787,16 +2715,15 @@
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
-      <c r="S68" s="6"/>
-      <c r="T68" s="1"/>
+      <c r="R68" s="6"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="6"/>
       <c r="U68" s="6"/>
-      <c r="V68" s="6"/>
+      <c r="V68" s="1"/>
       <c r="W68" s="1"/>
       <c r="X68" s="1"/>
-      <c r="Y68" s="1"/>
-    </row>
-    <row r="69" spans="1:25">
+    </row>
+    <row r="69" spans="1:24">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2814,16 +2741,15 @@
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-      <c r="S69" s="6"/>
-      <c r="T69" s="1"/>
+      <c r="R69" s="6"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="6"/>
       <c r="U69" s="6"/>
-      <c r="V69" s="6"/>
+      <c r="V69" s="1"/>
       <c r="W69" s="1"/>
       <c r="X69" s="1"/>
-      <c r="Y69" s="1"/>
-    </row>
-    <row r="70" spans="1:25">
+    </row>
+    <row r="70" spans="1:24">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2841,16 +2767,15 @@
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
-      <c r="S70" s="6"/>
-      <c r="T70" s="1"/>
+      <c r="R70" s="6"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="6"/>
       <c r="U70" s="6"/>
-      <c r="V70" s="6"/>
+      <c r="V70" s="1"/>
       <c r="W70" s="1"/>
       <c r="X70" s="1"/>
-      <c r="Y70" s="1"/>
-    </row>
-    <row r="71" spans="1:25">
+    </row>
+    <row r="71" spans="1:24">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2868,16 +2793,15 @@
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
-      <c r="R71" s="1"/>
-      <c r="S71" s="6"/>
-      <c r="T71" s="1"/>
+      <c r="R71" s="6"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="6"/>
       <c r="U71" s="6"/>
-      <c r="V71" s="6"/>
+      <c r="V71" s="1"/>
       <c r="W71" s="1"/>
       <c r="X71" s="1"/>
-      <c r="Y71" s="1"/>
-    </row>
-    <row r="72" spans="1:25">
+    </row>
+    <row r="72" spans="1:24">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2895,16 +2819,15 @@
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
-      <c r="R72" s="1"/>
-      <c r="S72" s="6"/>
-      <c r="T72" s="1"/>
+      <c r="R72" s="6"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="6"/>
       <c r="U72" s="6"/>
-      <c r="V72" s="6"/>
+      <c r="V72" s="1"/>
       <c r="W72" s="1"/>
       <c r="X72" s="1"/>
-      <c r="Y72" s="1"/>
-    </row>
-    <row r="73" spans="1:25">
+    </row>
+    <row r="73" spans="1:24">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2922,16 +2845,15 @@
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
-      <c r="R73" s="1"/>
-      <c r="S73" s="6"/>
-      <c r="T73" s="1"/>
+      <c r="R73" s="6"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="6"/>
       <c r="U73" s="6"/>
-      <c r="V73" s="6"/>
+      <c r="V73" s="1"/>
       <c r="W73" s="1"/>
       <c r="X73" s="1"/>
-      <c r="Y73" s="1"/>
-    </row>
-    <row r="74" spans="1:25">
+    </row>
+    <row r="74" spans="1:24">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2949,16 +2871,15 @@
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
-      <c r="S74" s="6"/>
-      <c r="T74" s="1"/>
+      <c r="R74" s="6"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="6"/>
       <c r="U74" s="6"/>
-      <c r="V74" s="6"/>
+      <c r="V74" s="1"/>
       <c r="W74" s="1"/>
       <c r="X74" s="1"/>
-      <c r="Y74" s="1"/>
-    </row>
-    <row r="75" spans="1:25">
+    </row>
+    <row r="75" spans="1:24">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2976,16 +2897,15 @@
       <c r="O75" s="1"/>
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
-      <c r="S75" s="6"/>
-      <c r="T75" s="1"/>
+      <c r="R75" s="6"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="6"/>
       <c r="U75" s="6"/>
-      <c r="V75" s="6"/>
+      <c r="V75" s="1"/>
       <c r="W75" s="1"/>
       <c r="X75" s="1"/>
-      <c r="Y75" s="1"/>
-    </row>
-    <row r="76" spans="1:25">
+    </row>
+    <row r="76" spans="1:24">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3003,16 +2923,15 @@
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
-      <c r="R76" s="1"/>
-      <c r="S76" s="6"/>
-      <c r="T76" s="1"/>
+      <c r="R76" s="6"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="6"/>
       <c r="U76" s="6"/>
-      <c r="V76" s="6"/>
+      <c r="V76" s="1"/>
       <c r="W76" s="1"/>
       <c r="X76" s="1"/>
-      <c r="Y76" s="1"/>
-    </row>
-    <row r="77" spans="1:25">
+    </row>
+    <row r="77" spans="1:24">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3030,16 +2949,15 @@
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
-      <c r="R77" s="1"/>
-      <c r="S77" s="6"/>
-      <c r="T77" s="1"/>
+      <c r="R77" s="6"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="6"/>
       <c r="U77" s="6"/>
-      <c r="V77" s="6"/>
+      <c r="V77" s="1"/>
       <c r="W77" s="1"/>
       <c r="X77" s="1"/>
-      <c r="Y77" s="1"/>
-    </row>
-    <row r="78" spans="1:25">
+    </row>
+    <row r="78" spans="1:24">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3057,16 +2975,15 @@
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
-      <c r="R78" s="1"/>
-      <c r="S78" s="6"/>
-      <c r="T78" s="1"/>
+      <c r="R78" s="6"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="6"/>
       <c r="U78" s="6"/>
-      <c r="V78" s="6"/>
+      <c r="V78" s="1"/>
       <c r="W78" s="1"/>
       <c r="X78" s="1"/>
-      <c r="Y78" s="1"/>
-    </row>
-    <row r="79" spans="1:25">
+    </row>
+    <row r="79" spans="1:24">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -3084,16 +3001,15 @@
       <c r="O79" s="1"/>
       <c r="P79" s="1"/>
       <c r="Q79" s="1"/>
-      <c r="R79" s="1"/>
-      <c r="S79" s="6"/>
-      <c r="T79" s="1"/>
+      <c r="R79" s="6"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="6"/>
       <c r="U79" s="6"/>
-      <c r="V79" s="6"/>
+      <c r="V79" s="1"/>
       <c r="W79" s="1"/>
       <c r="X79" s="1"/>
-      <c r="Y79" s="1"/>
-    </row>
-    <row r="80" spans="1:25">
+    </row>
+    <row r="80" spans="1:24">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -3111,16 +3027,15 @@
       <c r="O80" s="1"/>
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
-      <c r="R80" s="1"/>
-      <c r="S80" s="6"/>
-      <c r="T80" s="1"/>
+      <c r="R80" s="6"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="6"/>
       <c r="U80" s="6"/>
-      <c r="V80" s="6"/>
+      <c r="V80" s="1"/>
       <c r="W80" s="1"/>
       <c r="X80" s="1"/>
-      <c r="Y80" s="1"/>
-    </row>
-    <row r="81" spans="1:25">
+    </row>
+    <row r="81" spans="1:24">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -3138,16 +3053,15 @@
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
-      <c r="R81" s="1"/>
-      <c r="S81" s="6"/>
-      <c r="T81" s="1"/>
+      <c r="R81" s="6"/>
+      <c r="S81" s="1"/>
+      <c r="T81" s="6"/>
       <c r="U81" s="6"/>
-      <c r="V81" s="6"/>
+      <c r="V81" s="1"/>
       <c r="W81" s="1"/>
       <c r="X81" s="1"/>
-      <c r="Y81" s="1"/>
-    </row>
-    <row r="82" spans="1:25">
+    </row>
+    <row r="82" spans="1:24">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -3165,16 +3079,15 @@
       <c r="O82" s="1"/>
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
-      <c r="R82" s="1"/>
-      <c r="S82" s="6"/>
-      <c r="T82" s="1"/>
+      <c r="R82" s="6"/>
+      <c r="S82" s="1"/>
+      <c r="T82" s="6"/>
       <c r="U82" s="6"/>
-      <c r="V82" s="6"/>
+      <c r="V82" s="1"/>
       <c r="W82" s="1"/>
       <c r="X82" s="1"/>
-      <c r="Y82" s="1"/>
-    </row>
-    <row r="83" spans="1:25">
+    </row>
+    <row r="83" spans="1:24">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3192,16 +3105,15 @@
       <c r="O83" s="1"/>
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
-      <c r="R83" s="1"/>
-      <c r="S83" s="6"/>
-      <c r="T83" s="1"/>
+      <c r="R83" s="6"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="6"/>
       <c r="U83" s="6"/>
-      <c r="V83" s="6"/>
+      <c r="V83" s="1"/>
       <c r="W83" s="1"/>
       <c r="X83" s="1"/>
-      <c r="Y83" s="1"/>
-    </row>
-    <row r="84" spans="1:25">
+    </row>
+    <row r="84" spans="1:24">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3219,16 +3131,15 @@
       <c r="O84" s="1"/>
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
-      <c r="R84" s="1"/>
-      <c r="S84" s="6"/>
-      <c r="T84" s="1"/>
+      <c r="R84" s="6"/>
+      <c r="S84" s="1"/>
+      <c r="T84" s="6"/>
       <c r="U84" s="6"/>
-      <c r="V84" s="6"/>
+      <c r="V84" s="1"/>
       <c r="W84" s="1"/>
       <c r="X84" s="1"/>
-      <c r="Y84" s="1"/>
-    </row>
-    <row r="85" spans="1:25">
+    </row>
+    <row r="85" spans="1:24">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3246,16 +3157,15 @@
       <c r="O85" s="1"/>
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
-      <c r="R85" s="1"/>
-      <c r="S85" s="6"/>
-      <c r="T85" s="1"/>
+      <c r="R85" s="6"/>
+      <c r="S85" s="1"/>
+      <c r="T85" s="6"/>
       <c r="U85" s="6"/>
-      <c r="V85" s="6"/>
+      <c r="V85" s="1"/>
       <c r="W85" s="1"/>
       <c r="X85" s="1"/>
-      <c r="Y85" s="1"/>
-    </row>
-    <row r="86" spans="1:25">
+    </row>
+    <row r="86" spans="1:24">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3273,16 +3183,15 @@
       <c r="O86" s="1"/>
       <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
-      <c r="R86" s="1"/>
-      <c r="S86" s="6"/>
-      <c r="T86" s="1"/>
+      <c r="R86" s="6"/>
+      <c r="S86" s="1"/>
+      <c r="T86" s="6"/>
       <c r="U86" s="6"/>
-      <c r="V86" s="6"/>
+      <c r="V86" s="1"/>
       <c r="W86" s="1"/>
       <c r="X86" s="1"/>
-      <c r="Y86" s="1"/>
-    </row>
-    <row r="87" spans="1:25">
+    </row>
+    <row r="87" spans="1:24">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3300,16 +3209,15 @@
       <c r="O87" s="1"/>
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
-      <c r="R87" s="1"/>
-      <c r="S87" s="6"/>
-      <c r="T87" s="1"/>
+      <c r="R87" s="6"/>
+      <c r="S87" s="1"/>
+      <c r="T87" s="6"/>
       <c r="U87" s="6"/>
-      <c r="V87" s="6"/>
+      <c r="V87" s="1"/>
       <c r="W87" s="1"/>
       <c r="X87" s="1"/>
-      <c r="Y87" s="1"/>
-    </row>
-    <row r="88" spans="1:25">
+    </row>
+    <row r="88" spans="1:24">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3327,16 +3235,15 @@
       <c r="O88" s="1"/>
       <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
-      <c r="R88" s="1"/>
-      <c r="S88" s="6"/>
-      <c r="T88" s="1"/>
+      <c r="R88" s="6"/>
+      <c r="S88" s="1"/>
+      <c r="T88" s="6"/>
       <c r="U88" s="6"/>
-      <c r="V88" s="6"/>
+      <c r="V88" s="1"/>
       <c r="W88" s="1"/>
       <c r="X88" s="1"/>
-      <c r="Y88" s="1"/>
-    </row>
-    <row r="89" spans="1:25">
+    </row>
+    <row r="89" spans="1:24">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3354,16 +3261,15 @@
       <c r="O89" s="1"/>
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
-      <c r="R89" s="1"/>
-      <c r="S89" s="6"/>
-      <c r="T89" s="1"/>
+      <c r="R89" s="6"/>
+      <c r="S89" s="1"/>
+      <c r="T89" s="6"/>
       <c r="U89" s="6"/>
-      <c r="V89" s="6"/>
+      <c r="V89" s="1"/>
       <c r="W89" s="1"/>
       <c r="X89" s="1"/>
-      <c r="Y89" s="1"/>
-    </row>
-    <row r="90" spans="1:25">
+    </row>
+    <row r="90" spans="1:24">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3381,16 +3287,15 @@
       <c r="O90" s="1"/>
       <c r="P90" s="1"/>
       <c r="Q90" s="1"/>
-      <c r="R90" s="1"/>
-      <c r="S90" s="6"/>
-      <c r="T90" s="1"/>
+      <c r="R90" s="6"/>
+      <c r="S90" s="1"/>
+      <c r="T90" s="6"/>
       <c r="U90" s="6"/>
-      <c r="V90" s="6"/>
+      <c r="V90" s="1"/>
       <c r="W90" s="1"/>
       <c r="X90" s="1"/>
-      <c r="Y90" s="1"/>
-    </row>
-    <row r="91" spans="1:25">
+    </row>
+    <row r="91" spans="1:24">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3408,16 +3313,15 @@
       <c r="O91" s="1"/>
       <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
-      <c r="R91" s="1"/>
-      <c r="S91" s="6"/>
-      <c r="T91" s="1"/>
+      <c r="R91" s="6"/>
+      <c r="S91" s="1"/>
+      <c r="T91" s="6"/>
       <c r="U91" s="6"/>
-      <c r="V91" s="6"/>
+      <c r="V91" s="1"/>
       <c r="W91" s="1"/>
       <c r="X91" s="1"/>
-      <c r="Y91" s="1"/>
-    </row>
-    <row r="92" spans="1:25">
+    </row>
+    <row r="92" spans="1:24">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3435,16 +3339,15 @@
       <c r="O92" s="1"/>
       <c r="P92" s="1"/>
       <c r="Q92" s="1"/>
-      <c r="R92" s="1"/>
-      <c r="S92" s="6"/>
-      <c r="T92" s="1"/>
+      <c r="R92" s="6"/>
+      <c r="S92" s="1"/>
+      <c r="T92" s="6"/>
       <c r="U92" s="6"/>
-      <c r="V92" s="6"/>
+      <c r="V92" s="1"/>
       <c r="W92" s="1"/>
       <c r="X92" s="1"/>
-      <c r="Y92" s="1"/>
-    </row>
-    <row r="93" spans="1:25">
+    </row>
+    <row r="93" spans="1:24">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3462,16 +3365,15 @@
       <c r="O93" s="1"/>
       <c r="P93" s="1"/>
       <c r="Q93" s="1"/>
-      <c r="R93" s="1"/>
-      <c r="S93" s="6"/>
-      <c r="T93" s="1"/>
+      <c r="R93" s="6"/>
+      <c r="S93" s="1"/>
+      <c r="T93" s="6"/>
       <c r="U93" s="6"/>
-      <c r="V93" s="6"/>
+      <c r="V93" s="1"/>
       <c r="W93" s="1"/>
       <c r="X93" s="1"/>
-      <c r="Y93" s="1"/>
-    </row>
-    <row r="94" spans="1:25">
+    </row>
+    <row r="94" spans="1:24">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3489,16 +3391,15 @@
       <c r="O94" s="1"/>
       <c r="P94" s="1"/>
       <c r="Q94" s="1"/>
-      <c r="R94" s="1"/>
-      <c r="S94" s="6"/>
-      <c r="T94" s="1"/>
+      <c r="R94" s="6"/>
+      <c r="S94" s="1"/>
+      <c r="T94" s="6"/>
       <c r="U94" s="6"/>
-      <c r="V94" s="6"/>
+      <c r="V94" s="1"/>
       <c r="W94" s="1"/>
       <c r="X94" s="1"/>
-      <c r="Y94" s="1"/>
-    </row>
-    <row r="95" spans="1:25">
+    </row>
+    <row r="95" spans="1:24">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3516,16 +3417,15 @@
       <c r="O95" s="1"/>
       <c r="P95" s="1"/>
       <c r="Q95" s="1"/>
-      <c r="R95" s="1"/>
-      <c r="S95" s="6"/>
-      <c r="T95" s="1"/>
+      <c r="R95" s="6"/>
+      <c r="S95" s="1"/>
+      <c r="T95" s="6"/>
       <c r="U95" s="6"/>
-      <c r="V95" s="6"/>
+      <c r="V95" s="1"/>
       <c r="W95" s="1"/>
       <c r="X95" s="1"/>
-      <c r="Y95" s="1"/>
-    </row>
-    <row r="96" spans="1:25">
+    </row>
+    <row r="96" spans="1:24">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3543,16 +3443,15 @@
       <c r="O96" s="1"/>
       <c r="P96" s="1"/>
       <c r="Q96" s="1"/>
-      <c r="R96" s="1"/>
-      <c r="S96" s="6"/>
-      <c r="T96" s="1"/>
+      <c r="R96" s="6"/>
+      <c r="S96" s="1"/>
+      <c r="T96" s="6"/>
       <c r="U96" s="6"/>
-      <c r="V96" s="6"/>
+      <c r="V96" s="1"/>
       <c r="W96" s="1"/>
       <c r="X96" s="1"/>
-      <c r="Y96" s="1"/>
-    </row>
-    <row r="97" spans="1:25">
+    </row>
+    <row r="97" spans="1:24">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3570,16 +3469,15 @@
       <c r="O97" s="1"/>
       <c r="P97" s="1"/>
       <c r="Q97" s="1"/>
-      <c r="R97" s="1"/>
-      <c r="S97" s="6"/>
-      <c r="T97" s="1"/>
+      <c r="R97" s="6"/>
+      <c r="S97" s="1"/>
+      <c r="T97" s="6"/>
       <c r="U97" s="6"/>
-      <c r="V97" s="6"/>
+      <c r="V97" s="1"/>
       <c r="W97" s="1"/>
       <c r="X97" s="1"/>
-      <c r="Y97" s="1"/>
-    </row>
-    <row r="98" spans="1:25">
+    </row>
+    <row r="98" spans="1:24">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3597,16 +3495,15 @@
       <c r="O98" s="1"/>
       <c r="P98" s="1"/>
       <c r="Q98" s="1"/>
-      <c r="R98" s="1"/>
-      <c r="S98" s="6"/>
-      <c r="T98" s="1"/>
+      <c r="R98" s="6"/>
+      <c r="S98" s="1"/>
+      <c r="T98" s="6"/>
       <c r="U98" s="6"/>
-      <c r="V98" s="6"/>
+      <c r="V98" s="1"/>
       <c r="W98" s="1"/>
       <c r="X98" s="1"/>
-      <c r="Y98" s="1"/>
-    </row>
-    <row r="99" spans="1:25">
+    </row>
+    <row r="99" spans="1:24">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3626,14 +3523,13 @@
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
       <c r="S99" s="1"/>
-      <c r="T99" s="1"/>
+      <c r="T99" s="6"/>
       <c r="U99" s="6"/>
-      <c r="V99" s="6"/>
+      <c r="V99" s="1"/>
       <c r="W99" s="1"/>
       <c r="X99" s="1"/>
-      <c r="Y99" s="1"/>
-    </row>
-    <row r="100" spans="1:25">
+    </row>
+    <row r="100" spans="1:24">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3651,16 +3547,15 @@
       <c r="O100" s="1"/>
       <c r="P100" s="1"/>
       <c r="Q100" s="1"/>
-      <c r="R100" s="1"/>
-      <c r="S100" s="6"/>
-      <c r="T100" s="1"/>
+      <c r="R100" s="6"/>
+      <c r="S100" s="1"/>
+      <c r="T100" s="6"/>
       <c r="U100" s="6"/>
-      <c r="V100" s="6"/>
+      <c r="V100" s="1"/>
       <c r="W100" s="1"/>
       <c r="X100" s="1"/>
-      <c r="Y100" s="1"/>
-    </row>
-    <row r="101" spans="1:25">
+    </row>
+    <row r="101" spans="1:24">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3678,16 +3573,15 @@
       <c r="O101" s="1"/>
       <c r="P101" s="1"/>
       <c r="Q101" s="1"/>
-      <c r="R101" s="1"/>
-      <c r="S101" s="6"/>
-      <c r="T101" s="1"/>
+      <c r="R101" s="6"/>
+      <c r="S101" s="1"/>
+      <c r="T101" s="6"/>
       <c r="U101" s="6"/>
-      <c r="V101" s="6"/>
+      <c r="V101" s="1"/>
       <c r="W101" s="1"/>
       <c r="X101" s="1"/>
-      <c r="Y101" s="1"/>
-    </row>
-    <row r="102" spans="1:25">
+    </row>
+    <row r="102" spans="1:24">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3705,16 +3599,15 @@
       <c r="O102" s="1"/>
       <c r="P102" s="1"/>
       <c r="Q102" s="1"/>
-      <c r="R102" s="1"/>
-      <c r="S102" s="6"/>
-      <c r="T102" s="1"/>
+      <c r="R102" s="6"/>
+      <c r="S102" s="1"/>
+      <c r="T102" s="6"/>
       <c r="U102" s="6"/>
-      <c r="V102" s="6"/>
+      <c r="V102" s="1"/>
       <c r="W102" s="1"/>
       <c r="X102" s="1"/>
-      <c r="Y102" s="1"/>
-    </row>
-    <row r="103" spans="1:25">
+    </row>
+    <row r="103" spans="1:24">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3732,16 +3625,15 @@
       <c r="O103" s="1"/>
       <c r="P103" s="1"/>
       <c r="Q103" s="1"/>
-      <c r="R103" s="1"/>
-      <c r="S103" s="6"/>
-      <c r="T103" s="1"/>
+      <c r="R103" s="6"/>
+      <c r="S103" s="1"/>
+      <c r="T103" s="6"/>
       <c r="U103" s="6"/>
-      <c r="V103" s="6"/>
+      <c r="V103" s="1"/>
       <c r="W103" s="1"/>
       <c r="X103" s="1"/>
-      <c r="Y103" s="1"/>
-    </row>
-    <row r="104" spans="1:25">
+    </row>
+    <row r="104" spans="1:24">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3759,16 +3651,15 @@
       <c r="O104" s="1"/>
       <c r="P104" s="1"/>
       <c r="Q104" s="1"/>
-      <c r="R104" s="1"/>
-      <c r="S104" s="6"/>
-      <c r="T104" s="1"/>
+      <c r="R104" s="6"/>
+      <c r="S104" s="1"/>
+      <c r="T104" s="6"/>
       <c r="U104" s="6"/>
-      <c r="V104" s="6"/>
+      <c r="V104" s="1"/>
       <c r="W104" s="1"/>
       <c r="X104" s="1"/>
-      <c r="Y104" s="1"/>
-    </row>
-    <row r="105" spans="1:25">
+    </row>
+    <row r="105" spans="1:24">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3788,14 +3679,13 @@
       <c r="Q105" s="1"/>
       <c r="R105" s="1"/>
       <c r="S105" s="1"/>
-      <c r="T105" s="1"/>
+      <c r="T105" s="6"/>
       <c r="U105" s="6"/>
-      <c r="V105" s="6"/>
+      <c r="V105" s="1"/>
       <c r="W105" s="1"/>
       <c r="X105" s="1"/>
-      <c r="Y105" s="1"/>
-    </row>
-    <row r="106" spans="1:25" ht="49.5" customHeight="1">
+    </row>
+    <row r="106" spans="1:24" ht="49.5" customHeight="1">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3813,16 +3703,15 @@
       <c r="O106" s="1"/>
       <c r="P106" s="1"/>
       <c r="Q106" s="1"/>
-      <c r="R106" s="1"/>
-      <c r="S106" s="6"/>
-      <c r="T106" s="1"/>
+      <c r="R106" s="6"/>
+      <c r="S106" s="1"/>
+      <c r="T106" s="6"/>
       <c r="U106" s="6"/>
-      <c r="V106" s="6"/>
+      <c r="V106" s="1"/>
       <c r="W106" s="1"/>
       <c r="X106" s="1"/>
-      <c r="Y106" s="1"/>
-    </row>
-    <row r="107" spans="1:25" ht="49.5" customHeight="1">
+    </row>
+    <row r="107" spans="1:24" ht="49.5" customHeight="1">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3840,101 +3729,100 @@
       <c r="O107" s="1"/>
       <c r="P107" s="1"/>
       <c r="Q107" s="1"/>
-      <c r="R107" s="1"/>
-      <c r="S107" s="6"/>
-      <c r="T107" s="1"/>
+      <c r="R107" s="6"/>
+      <c r="S107" s="1"/>
+      <c r="T107" s="6"/>
       <c r="U107" s="6"/>
-      <c r="V107" s="6"/>
+      <c r="V107" s="1"/>
       <c r="W107" s="1"/>
       <c r="X107" s="1"/>
-      <c r="Y107" s="1"/>
-    </row>
-    <row r="108" spans="1:25" s="1" customFormat="1">
+    </row>
+    <row r="108" spans="1:24" s="1" customFormat="1">
       <c r="E108" s="2"/>
       <c r="F108" s="3"/>
       <c r="G108" s="4"/>
       <c r="H108" s="5"/>
       <c r="I108" s="2"/>
-      <c r="S108" s="6"/>
+      <c r="R108" s="6"/>
+      <c r="T108" s="6"/>
       <c r="U108" s="6"/>
-      <c r="V108" s="6"/>
-    </row>
-    <row r="109" spans="1:25" s="1" customFormat="1">
+    </row>
+    <row r="109" spans="1:24" s="1" customFormat="1">
       <c r="E109" s="2"/>
       <c r="F109" s="3"/>
       <c r="G109" s="4"/>
       <c r="H109" s="5"/>
       <c r="I109" s="2"/>
-      <c r="S109" s="6"/>
+      <c r="R109" s="6"/>
+      <c r="T109" s="6"/>
       <c r="U109" s="6"/>
-      <c r="V109" s="6"/>
-    </row>
-    <row r="110" spans="1:25" s="1" customFormat="1">
+    </row>
+    <row r="110" spans="1:24" s="1" customFormat="1">
       <c r="E110" s="2"/>
       <c r="F110" s="3"/>
       <c r="G110" s="4"/>
       <c r="H110" s="5"/>
       <c r="I110" s="2"/>
-      <c r="S110" s="6"/>
+      <c r="R110" s="6"/>
+      <c r="T110" s="6"/>
       <c r="U110" s="6"/>
-      <c r="V110" s="6"/>
-    </row>
-    <row r="111" spans="1:25" s="1" customFormat="1">
+    </row>
+    <row r="111" spans="1:24" s="1" customFormat="1">
       <c r="E111" s="2"/>
       <c r="F111" s="3"/>
       <c r="G111" s="4"/>
       <c r="H111" s="5"/>
       <c r="I111" s="2"/>
-      <c r="S111" s="6"/>
+      <c r="R111" s="6"/>
+      <c r="T111" s="6"/>
       <c r="U111" s="6"/>
-      <c r="V111" s="6"/>
-    </row>
-    <row r="112" spans="1:25" s="1" customFormat="1">
+    </row>
+    <row r="112" spans="1:24" s="1" customFormat="1">
       <c r="E112" s="2"/>
       <c r="F112" s="3"/>
       <c r="G112" s="4"/>
       <c r="H112" s="5"/>
       <c r="I112" s="2"/>
-      <c r="S112" s="6"/>
+      <c r="R112" s="6"/>
+      <c r="T112" s="6"/>
       <c r="U112" s="6"/>
-      <c r="V112" s="6"/>
-    </row>
-    <row r="113" spans="5:22" s="1" customFormat="1">
+    </row>
+    <row r="113" spans="5:21" s="1" customFormat="1">
       <c r="E113" s="2"/>
       <c r="F113" s="3"/>
       <c r="G113" s="4"/>
       <c r="H113" s="5"/>
       <c r="I113" s="2"/>
-      <c r="S113" s="6"/>
+      <c r="R113" s="6"/>
+      <c r="T113" s="6"/>
       <c r="U113" s="6"/>
-      <c r="V113" s="6"/>
-    </row>
-    <row r="114" spans="5:22" s="1" customFormat="1">
+    </row>
+    <row r="114" spans="5:21" s="1" customFormat="1">
       <c r="E114" s="2"/>
       <c r="F114" s="3"/>
       <c r="G114" s="4"/>
       <c r="H114" s="5"/>
       <c r="I114" s="2"/>
-      <c r="S114" s="6"/>
+      <c r="R114" s="6"/>
+      <c r="T114" s="6"/>
       <c r="U114" s="6"/>
-      <c r="V114" s="6"/>
-    </row>
-    <row r="115" spans="5:22" s="1" customFormat="1">
+    </row>
+    <row r="115" spans="5:21" s="1" customFormat="1">
       <c r="E115" s="2"/>
       <c r="F115" s="3"/>
       <c r="G115" s="4"/>
       <c r="H115" s="5"/>
       <c r="I115" s="2"/>
-      <c r="S115" s="6"/>
+      <c r="R115" s="6"/>
+      <c r="T115" s="6"/>
       <c r="U115" s="6"/>
-      <c r="V115" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A2:Y115">
     <sortCondition ref="E2:E115"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:V115 S2:S107">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:U115 R2:R107">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3960,55 +3848,55 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>